<commit_message>
la til mandagens resultater
</commit_message>
<xml_diff>
--- a/treningsdagbok.xlsx
+++ b/treningsdagbok.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bendik Bærbar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bendik Bærbar\treningsdagbok\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="8730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18768" windowHeight="8736"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
   <si>
     <t>dato</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>må ta knebøy igjen</t>
+  </si>
+  <si>
+    <t>ta benk og knebøy på nytt, glemte at jeg skulle ta 62,5</t>
   </si>
 </sst>
 </file>
@@ -708,6 +711,9 @@
                 <c:pt idx="70">
                   <c:v>42895</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>42905</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -841,6 +847,9 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="71">
                   <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
@@ -1340,6 +1349,9 @@
                 <c:pt idx="70">
                   <c:v>42895</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>42905</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1903,6 +1915,9 @@
                 <c:pt idx="70">
                   <c:v>42895</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>42905</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1980,6 +1995,9 @@
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2478,6 +2496,9 @@
                 <c:pt idx="70">
                   <c:v>42895</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>42905</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3044,6 +3065,9 @@
                 <c:pt idx="70">
                   <c:v>42895</c:v>
                 </c:pt>
+                <c:pt idx="71">
+                  <c:v>42905</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3117,6 +3141,9 @@
                   <c:v>57.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="71">
                   <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
@@ -6573,20 +6600,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -6621,7 +6648,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>42669</v>
@@ -6642,7 +6669,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>42671</v>
@@ -6663,7 +6690,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>42674</v>
@@ -6684,7 +6711,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>42676</v>
@@ -6705,7 +6732,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>42678</v>
@@ -6726,7 +6753,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>75</v>
       </c>
@@ -6749,7 +6776,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>70</v>
       </c>
@@ -6774,7 +6801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>90</v>
       </c>
@@ -6799,7 +6826,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>65</v>
       </c>
@@ -6822,7 +6849,7 @@
       </c>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>65</v>
       </c>
@@ -6845,7 +6872,7 @@
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>80</v>
       </c>
@@ -6870,7 +6897,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>120</v>
       </c>
@@ -6889,7 +6916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>60</v>
       </c>
@@ -6918,7 +6945,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>70</v>
       </c>
@@ -6943,7 +6970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>85</v>
       </c>
@@ -6968,7 +6995,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>50</v>
       </c>
@@ -6993,7 +7020,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>70</v>
       </c>
@@ -7020,7 +7047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>60</v>
       </c>
@@ -7047,7 +7074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>65</v>
       </c>
@@ -7074,7 +7101,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>60</v>
       </c>
@@ -7095,7 +7122,7 @@
       </c>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>75</v>
       </c>
@@ -7118,7 +7145,7 @@
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>65</v>
       </c>
@@ -7145,7 +7172,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>80</v>
       </c>
@@ -7170,7 +7197,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>50</v>
       </c>
@@ -7195,7 +7222,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>60</v>
       </c>
@@ -7220,7 +7247,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>70</v>
       </c>
@@ -7247,7 +7274,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>70</v>
       </c>
@@ -7274,7 +7301,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45</v>
       </c>
@@ -7297,7 +7324,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>60</v>
       </c>
@@ -7320,7 +7347,7 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>80</v>
       </c>
@@ -7347,7 +7374,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>80</v>
       </c>
@@ -7374,7 +7401,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>60</v>
       </c>
@@ -7397,7 +7424,7 @@
       </c>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>75</v>
       </c>
@@ -7424,7 +7451,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>60</v>
       </c>
@@ -7447,7 +7474,7 @@
       </c>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>60</v>
       </c>
@@ -7472,7 +7499,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>70</v>
       </c>
@@ -7499,7 +7526,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>65</v>
       </c>
@@ -7522,7 +7549,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>30</v>
       </c>
@@ -7545,7 +7572,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>55</v>
       </c>
@@ -7570,7 +7597,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>60</v>
       </c>
@@ -7595,7 +7622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>60</v>
       </c>
@@ -7614,7 +7641,7 @@
       </c>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>65</v>
       </c>
@@ -7641,7 +7668,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>300</v>
       </c>
@@ -7662,7 +7689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>70</v>
       </c>
@@ -7689,7 +7716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>55</v>
       </c>
@@ -7712,7 +7739,7 @@
       </c>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>65</v>
       </c>
@@ -7741,7 +7768,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>35</v>
       </c>
@@ -7764,7 +7791,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>65</v>
       </c>
@@ -7789,7 +7816,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>55</v>
       </c>
@@ -7814,7 +7841,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>80</v>
       </c>
@@ -7837,7 +7864,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>90</v>
       </c>
@@ -7856,7 +7883,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>30</v>
       </c>
@@ -7877,7 +7904,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>65</v>
       </c>
@@ -7900,7 +7927,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>40</v>
       </c>
@@ -7919,7 +7946,7 @@
       </c>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>75</v>
       </c>
@@ -7944,7 +7971,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45</v>
       </c>
@@ -7965,7 +7992,7 @@
       </c>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>120</v>
       </c>
@@ -7984,7 +8011,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>75</v>
       </c>
@@ -8009,7 +8036,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>30</v>
       </c>
@@ -8032,7 +8059,7 @@
       </c>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>55</v>
       </c>
@@ -8049,7 +8076,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>55</v>
       </c>
@@ -8070,7 +8097,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>40</v>
       </c>
@@ -8093,7 +8120,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>60</v>
       </c>
@@ -8116,7 +8143,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>65</v>
       </c>
@@ -8141,7 +8168,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>120</v>
       </c>
@@ -8162,7 +8189,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f>65+190</f>
         <v>255</v>
@@ -8192,7 +8219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>65</v>
       </c>
@@ -8217,7 +8244,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>60</v>
       </c>
@@ -8240,7 +8267,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>65</v>
       </c>
@@ -8265,7 +8292,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>55</v>
       </c>
@@ -8286,7 +8313,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>55</v>
       </c>
@@ -8311,20 +8338,32 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>60</v>
+      </c>
+      <c r="B76" s="2">
+        <v>42905</v>
+      </c>
+      <c r="C76" s="1">
+        <v>115</v>
+      </c>
+      <c r="D76" s="1">
+        <v>85</v>
+      </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="G76" s="1">
+        <v>60</v>
+      </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -8337,7 +8376,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -8350,7 +8389,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -8363,7 +8402,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -8376,7 +8415,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -8389,7 +8428,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -8402,7 +8441,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -8415,7 +8454,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -8428,7 +8467,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -8441,7 +8480,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -8454,7 +8493,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -8467,7 +8506,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -8480,7 +8519,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -8493,7 +8532,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -8506,7 +8545,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -8519,7 +8558,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -8532,7 +8571,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -8545,7 +8584,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -8558,7 +8597,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -8571,7 +8610,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -8584,7 +8623,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -8597,7 +8636,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -8610,7 +8649,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -8623,7 +8662,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -8636,7 +8675,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -8649,7 +8688,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -8662,7 +8701,7 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -8675,7 +8714,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -8688,7 +8727,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -8701,7 +8740,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -8714,7 +8753,7 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -8727,7 +8766,7 @@
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -8740,7 +8779,7 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -8753,7 +8792,7 @@
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -8766,7 +8805,7 @@
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -8779,7 +8818,7 @@
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -8792,7 +8831,7 @@
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -8805,7 +8844,7 @@
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -8818,7 +8857,7 @@
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -8831,7 +8870,7 @@
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -8844,7 +8883,7 @@
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -8857,7 +8896,7 @@
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -8870,7 +8909,7 @@
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -8883,7 +8922,7 @@
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -8896,7 +8935,7 @@
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -8909,7 +8948,7 @@
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -8922,7 +8961,7 @@
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -8935,7 +8974,7 @@
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -8948,7 +8987,7 @@
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -8961,7 +9000,7 @@
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -8974,7 +9013,7 @@
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -8987,7 +9026,7 @@
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -9000,7 +9039,7 @@
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -9013,7 +9052,7 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -9026,7 +9065,7 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>

</xml_diff>